<commit_message>
Fix: length and range at S9(9) is wrong
Signed-off-by: Janos Varga <113785741+vargajb@users.noreply.github.com>
Signed-off-by: pathange-s <sainatharao@gmail.com>
</commit_message>
<xml_diff>
--- a/COBOL Programming Course #3 - Advanced Topics/Images/binary-ranges.xlsx
+++ b/COBOL Programming Course #3 - Advanced Topics/Images/binary-ranges.xlsx
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="105" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="106" uniqueCount="31">
   <si>
     <t>Range</t>
   </si>
@@ -680,7 +680,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="35">
+  <cellXfs count="32">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -746,15 +746,6 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="17" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="7" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="10" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="2" borderId="7" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1126,10 +1117,10 @@
       <c r="A2" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="33" t="s">
+      <c r="B2" s="30" t="s">
         <v>2</v>
       </c>
-      <c r="C2" s="34" t="s">
+      <c r="C2" s="31" t="s">
         <v>26</v>
       </c>
       <c r="D2" s="4" t="s">
@@ -1141,8 +1132,8 @@
       <c r="A3" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="B3" s="28"/>
-      <c r="C3" s="30"/>
+      <c r="B3" s="25"/>
+      <c r="C3" s="27"/>
       <c r="D3" s="7" t="s">
         <v>5</v>
       </c>
@@ -1152,10 +1143,10 @@
       <c r="A4" s="6" t="s">
         <v>1</v>
       </c>
-      <c r="B4" s="28" t="s">
+      <c r="B4" s="25" t="s">
         <v>6</v>
       </c>
-      <c r="C4" s="30"/>
+      <c r="C4" s="27"/>
       <c r="D4" s="9" t="s">
         <v>7</v>
       </c>
@@ -1165,8 +1156,8 @@
       <c r="A5" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="B5" s="28"/>
-      <c r="C5" s="30"/>
+      <c r="B5" s="25"/>
+      <c r="C5" s="27"/>
       <c r="D5" s="9" t="s">
         <v>8</v>
       </c>
@@ -1176,10 +1167,10 @@
       <c r="A6" s="6" t="s">
         <v>1</v>
       </c>
-      <c r="B6" s="28" t="s">
+      <c r="B6" s="25" t="s">
         <v>9</v>
       </c>
-      <c r="C6" s="30"/>
+      <c r="C6" s="27"/>
       <c r="D6" s="7" t="s">
         <v>10</v>
       </c>
@@ -1189,8 +1180,8 @@
       <c r="A7" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="B7" s="28"/>
-      <c r="C7" s="30"/>
+      <c r="B7" s="25"/>
+      <c r="C7" s="27"/>
       <c r="D7" s="7" t="s">
         <v>5</v>
       </c>
@@ -1200,10 +1191,10 @@
       <c r="A8" s="6" t="s">
         <v>1</v>
       </c>
-      <c r="B8" s="28" t="s">
+      <c r="B8" s="25" t="s">
         <v>11</v>
       </c>
-      <c r="C8" s="30"/>
+      <c r="C8" s="27"/>
       <c r="D8" s="7" t="s">
         <v>12</v>
       </c>
@@ -1213,8 +1204,8 @@
       <c r="A9" s="10" t="s">
         <v>4</v>
       </c>
-      <c r="B9" s="32"/>
-      <c r="C9" s="31"/>
+      <c r="B9" s="29"/>
+      <c r="C9" s="28"/>
       <c r="D9" s="11" t="s">
         <v>5</v>
       </c>
@@ -1226,10 +1217,10 @@
       <c r="A10" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="B10" s="33" t="s">
+      <c r="B10" s="30" t="s">
         <v>13</v>
       </c>
-      <c r="C10" s="34" t="s">
+      <c r="C10" s="31" t="s">
         <v>27</v>
       </c>
       <c r="D10" s="4" t="s">
@@ -1241,12 +1232,12 @@
       <c r="A11" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="B11" s="28"/>
-      <c r="C11" s="30"/>
+      <c r="B11" s="25"/>
+      <c r="C11" s="27"/>
       <c r="D11" s="7" t="s">
         <v>15</v>
       </c>
-      <c r="E11" s="26" t="s">
+      <c r="E11" s="23" t="s">
         <v>30</v>
       </c>
     </row>
@@ -1254,10 +1245,10 @@
       <c r="A12" s="6" t="s">
         <v>1</v>
       </c>
-      <c r="B12" s="28" t="s">
+      <c r="B12" s="25" t="s">
         <v>16</v>
       </c>
-      <c r="C12" s="30"/>
+      <c r="C12" s="27"/>
       <c r="D12" s="7" t="s">
         <v>17</v>
       </c>
@@ -1267,8 +1258,8 @@
       <c r="A13" s="10" t="s">
         <v>4</v>
       </c>
-      <c r="B13" s="32"/>
-      <c r="C13" s="31"/>
+      <c r="B13" s="29"/>
+      <c r="C13" s="28"/>
       <c r="D13" s="11" t="s">
         <v>15</v>
       </c>
@@ -1278,10 +1269,10 @@
       <c r="A14" s="15" t="s">
         <v>1</v>
       </c>
-      <c r="B14" s="27" t="s">
+      <c r="B14" s="24" t="s">
         <v>21</v>
       </c>
-      <c r="C14" s="29" t="s">
+      <c r="C14" s="26" t="s">
         <v>28</v>
       </c>
       <c r="D14" s="16" t="s">
@@ -1293,8 +1284,8 @@
       <c r="A15" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="B15" s="28"/>
-      <c r="C15" s="30"/>
+      <c r="B15" s="25"/>
+      <c r="C15" s="27"/>
       <c r="D15" s="7" t="s">
         <v>20</v>
       </c>
@@ -1304,10 +1295,10 @@
       <c r="A16" s="6" t="s">
         <v>1</v>
       </c>
-      <c r="B16" s="28" t="s">
+      <c r="B16" s="25" t="s">
         <v>18</v>
       </c>
-      <c r="C16" s="30"/>
+      <c r="C16" s="27"/>
       <c r="D16" s="7" t="s">
         <v>19</v>
       </c>
@@ -1317,8 +1308,8 @@
       <c r="A17" s="10" t="s">
         <v>4</v>
       </c>
-      <c r="B17" s="32"/>
-      <c r="C17" s="31"/>
+      <c r="B17" s="29"/>
+      <c r="C17" s="28"/>
       <c r="D17" s="11" t="s">
         <v>20</v>
       </c>
@@ -1377,10 +1368,10 @@
       <c r="A2" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="33" t="s">
+      <c r="B2" s="30" t="s">
         <v>2</v>
       </c>
-      <c r="C2" s="34" t="s">
+      <c r="C2" s="31" t="s">
         <v>26</v>
       </c>
       <c r="D2" s="4" t="s">
@@ -1392,8 +1383,8 @@
       <c r="A3" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="B3" s="28"/>
-      <c r="C3" s="30"/>
+      <c r="B3" s="25"/>
+      <c r="C3" s="27"/>
       <c r="D3" s="7" t="s">
         <v>5</v>
       </c>
@@ -1403,10 +1394,10 @@
       <c r="A4" s="6" t="s">
         <v>1</v>
       </c>
-      <c r="B4" s="28" t="s">
+      <c r="B4" s="25" t="s">
         <v>6</v>
       </c>
-      <c r="C4" s="30"/>
+      <c r="C4" s="27"/>
       <c r="D4" s="9" t="s">
         <v>7</v>
       </c>
@@ -1416,8 +1407,8 @@
       <c r="A5" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="B5" s="28"/>
-      <c r="C5" s="30"/>
+      <c r="B5" s="25"/>
+      <c r="C5" s="27"/>
       <c r="D5" s="9" t="s">
         <v>8</v>
       </c>
@@ -1427,10 +1418,10 @@
       <c r="A6" s="6" t="s">
         <v>1</v>
       </c>
-      <c r="B6" s="28" t="s">
+      <c r="B6" s="25" t="s">
         <v>9</v>
       </c>
-      <c r="C6" s="30"/>
+      <c r="C6" s="27"/>
       <c r="D6" s="7" t="s">
         <v>10</v>
       </c>
@@ -1440,8 +1431,8 @@
       <c r="A7" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="B7" s="28"/>
-      <c r="C7" s="30"/>
+      <c r="B7" s="25"/>
+      <c r="C7" s="27"/>
       <c r="D7" s="7" t="s">
         <v>5</v>
       </c>
@@ -1451,10 +1442,10 @@
       <c r="A8" s="6" t="s">
         <v>1</v>
       </c>
-      <c r="B8" s="28" t="s">
+      <c r="B8" s="25" t="s">
         <v>11</v>
       </c>
-      <c r="C8" s="30"/>
+      <c r="C8" s="27"/>
       <c r="D8" s="7" t="s">
         <v>12</v>
       </c>
@@ -1464,8 +1455,8 @@
       <c r="A9" s="10" t="s">
         <v>4</v>
       </c>
-      <c r="B9" s="32"/>
-      <c r="C9" s="31"/>
+      <c r="B9" s="29"/>
+      <c r="C9" s="28"/>
       <c r="D9" s="11" t="s">
         <v>5</v>
       </c>
@@ -1524,10 +1515,10 @@
       <c r="A2" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="33" t="s">
+      <c r="B2" s="30" t="s">
         <v>13</v>
       </c>
-      <c r="C2" s="34" t="s">
+      <c r="C2" s="31" t="s">
         <v>27</v>
       </c>
       <c r="D2" s="4" t="s">
@@ -1539,12 +1530,12 @@
       <c r="A3" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="B3" s="28"/>
-      <c r="C3" s="30"/>
+      <c r="B3" s="25"/>
+      <c r="C3" s="27"/>
       <c r="D3" s="7" t="s">
         <v>15</v>
       </c>
-      <c r="E3" s="26" t="s">
+      <c r="E3" s="23" t="s">
         <v>30</v>
       </c>
     </row>
@@ -1552,10 +1543,10 @@
       <c r="A4" s="6" t="s">
         <v>1</v>
       </c>
-      <c r="B4" s="28" t="s">
+      <c r="B4" s="25" t="s">
         <v>16</v>
       </c>
-      <c r="C4" s="30"/>
+      <c r="C4" s="27"/>
       <c r="D4" s="7" t="s">
         <v>17</v>
       </c>
@@ -1565,8 +1556,8 @@
       <c r="A5" s="10" t="s">
         <v>4</v>
       </c>
-      <c r="B5" s="32"/>
-      <c r="C5" s="31"/>
+      <c r="B5" s="29"/>
+      <c r="C5" s="28"/>
       <c r="D5" s="11" t="s">
         <v>15</v>
       </c>
@@ -1589,7 +1580,7 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D5"/>
+  <dimension ref="A1:E5"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0"/>
   </sheetViews>
@@ -1599,9 +1590,10 @@
     <col min="2" max="2" width="5.5" customWidth="1"/>
     <col min="3" max="3" width="8" customWidth="1"/>
     <col min="4" max="4" width="24.5" customWidth="1"/>
+    <col min="5" max="5" width="35" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="30.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" ht="30.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A1" s="21"/>
       <c r="B1" s="22" t="s">
         <v>23</v>
@@ -1609,55 +1601,62 @@
       <c r="C1" s="18" t="s">
         <v>24</v>
       </c>
-      <c r="D1" s="19" t="s">
+      <c r="D1" s="18" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="2" spans="1:4" ht="28.5" x14ac:dyDescent="0.2">
+      <c r="E1" s="19" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" ht="28.5" x14ac:dyDescent="0.3">
       <c r="A2" s="15" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="27" t="s">
+      <c r="B2" s="24" t="s">
         <v>21</v>
       </c>
-      <c r="C2" s="29" t="s">
+      <c r="C2" s="26" t="s">
         <v>28</v>
       </c>
-      <c r="D2" s="23" t="s">
+      <c r="D2" s="16" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="3" spans="1:4" ht="28.5" x14ac:dyDescent="0.2">
+      <c r="E2" s="17"/>
+    </row>
+    <row r="3" spans="1:5" ht="28.5" x14ac:dyDescent="0.3">
       <c r="A3" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="B3" s="28"/>
-      <c r="C3" s="30"/>
-      <c r="D3" s="24" t="s">
+      <c r="B3" s="25"/>
+      <c r="C3" s="27"/>
+      <c r="D3" s="7" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="4" spans="1:4" ht="28.5" x14ac:dyDescent="0.2">
+      <c r="E3" s="8"/>
+    </row>
+    <row r="4" spans="1:5" ht="28.5" x14ac:dyDescent="0.3">
       <c r="A4" s="6" t="s">
         <v>1</v>
       </c>
-      <c r="B4" s="28" t="s">
+      <c r="B4" s="25" t="s">
         <v>18</v>
       </c>
-      <c r="C4" s="30"/>
-      <c r="D4" s="24" t="s">
+      <c r="C4" s="27"/>
+      <c r="D4" s="7" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="5" spans="1:4" ht="29.25" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="E4" s="8"/>
+    </row>
+    <row r="5" spans="1:5" ht="29.25" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A5" s="10" t="s">
         <v>4</v>
       </c>
-      <c r="B5" s="32"/>
-      <c r="C5" s="31"/>
-      <c r="D5" s="25" t="s">
+      <c r="B5" s="29"/>
+      <c r="C5" s="28"/>
+      <c r="D5" s="11" t="s">
         <v>20</v>
       </c>
+      <c r="E5" s="14"/>
     </row>
   </sheetData>
   <mergeCells count="3">

</xml_diff>